<commit_message>
refactor: Integrate cascade events into unified JSON structure
</commit_message>
<xml_diff>
--- a/data/game_initial_values_with_formulas.xlsx
+++ b/data/game_initial_values_with_formulas.xlsx
@@ -18,6 +18,12 @@
     <sheet name="Test_Constants" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="UI_Constants" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Performance_Constants" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Metric_Ranges" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Game_Flow_Constants" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Probability_Constants" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Threshold_Constants" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Storyteller_Constants" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Technical_Constants" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1050,6 +1056,1131 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric_Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Min_Value</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Max_Value</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Default_Value</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MONEY</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>MONEY의 허용 범위 및 기본값</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>REPUTATION</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D3" t="n">
+        <v>50</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>REPUTATION의 허용 범위 및 기본값</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>HAPPINESS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D4" t="n">
+        <v>50</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>HAPPINESS의 허용 범위 및 기본값</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SUFFERING</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>SUFFERING의 허용 범위 및 기본값</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>INVENTORY</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>100</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>INVENTORY의 허용 범위 및 기본값</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>STAFF_FATIGUE</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>100</v>
+      </c>
+      <c r="D7" t="n">
+        <v>30</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>STAFF_FATIGUE의 허용 범위 및 기본값</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>FACILITY</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" t="n">
+        <v>80</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>FACILITY의 허용 범위 및 기본값</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DEMAND</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>60</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>DEMAND의 허용 범위 및 기본값</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Key</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MAX_ACTIONS_PER_DAY</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>game_flow</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>하루 최대 행동 횟수</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DEFAULT_GAME_LENGTH</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>30</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>game_flow</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>기본 게임 길이(일)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>DEFAULT_TOTAL_DAYS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>730</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>game_flow</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>기본 게임 총 일수</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DEFAULT_COOLDOWN_DAYS</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>game_flow</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>기본 쿨다운 일수</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Key</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>PROBABILITY_LOW_THRESHOLD</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>probability</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>낮은 확률 임계값</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>PROBABILITY_HIGH_THRESHOLD</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>probability</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>높은 확률 임계값</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>DEFAULT_PROBABILITY</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>probability</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>기본 확률값</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DEFAULT_SEVERITY</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>probability</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>기본 심각도</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Key</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MONEY_LOW_THRESHOLD</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3000</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>thresholds</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>자금 부족 기준</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>MONEY_HIGH_THRESHOLD</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15000</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>thresholds</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>자금 풍부 기준</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>REPUTATION_LOW_THRESHOLD</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>30</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>thresholds</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>평판 위험 기준</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>REPUTATION_HIGH_THRESHOLD</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>70</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>thresholds</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>평판 우수 기준</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>HAPPINESS_LOW_THRESHOLD</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>thresholds</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>행복 위험 기준</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>HAPPINESS_HIGH_THRESHOLD</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>70</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>thresholds</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>행복 우수 기준</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>REPUTATION_BASELINE</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>50</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>thresholds</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>평판 기준점</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Key</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MIN_METRICS_HISTORY_FOR_TREND</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>storyteller</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>추세 분석을 위한 최소 히스토리 개수</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>RECENT_HISTORY_WINDOW</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>storyteller</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>최근 히스토리 분석 윈도우 크기</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MINIMUM_TREND_POINTS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>storyteller</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>트렌드 분석에 필요한 최소 데이터 포인트</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SITUATION_POSITIVE_THRESHOLD</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>storyteller</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>긍정적 상황 판단 임계값</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SITUATION_NEGATIVE_THRESHOLD</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>storyteller</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>부정적 상황 판단 임계값</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TRADEOFF_BALANCE_THRESHOLD</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>storyteller</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>트레이드오프 불균형 감지 임계값</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>GAME_PROGRESSION_MID_POINT</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>storyteller</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>게임 진행도 중간점</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>PATTERN_SCORE_TOLERANCE</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>storyteller</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>패턴 점수 허용 오차</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>COMPLEXITY_BONUS_MULTIPLIER</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>storyteller</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>복잡성 보너스 배수</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Key</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>FLOAT_EPSILON</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>technical</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>부동소수점 비교 오차 허용 범위</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SCORE_THRESHOLD_HIGH</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>technical</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>높은 점수 임계값</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>SCORE_THRESHOLD_MEDIUM</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>technical</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>중간 점수 임계값</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -1387,7 +2518,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1413,11 +2544,6 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Formula</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>Description</t>
         </is>
       </c>
@@ -1425,250 +2551,240 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Money</t>
+          <t>MONEY</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Happiness</t>
+          <t>HAPPINESS</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.3</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>돈이 많을수록 행복도 감소</t>
+        <v>-0.5</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>MONEY 상승 시 HAPPINESS 하락</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Money</t>
+          <t>MONEY</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Staff_Fatigue</t>
+          <t>STAFF_FATIGUE</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>돈이 많을수록 피로도 증가</t>
+        <v>-0.5</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>MONEY 상승 시 STAFF_FATIGUE 하락</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>REPUTATION</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Money</t>
+          <t>MONEY</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.25</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>평판이 높을수록 돈 감소</t>
+        <v>-0.5</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>REPUTATION 상승 시 MONEY 하락</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>REPUTATION</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Staff_Fatigue</t>
+          <t>STAFF_FATIGUE</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>평판이 높을수록 피로도 증가</t>
+        <v>-0.5</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>REPUTATION 상승 시 STAFF_FATIGUE 하락</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Happiness</t>
+          <t>HAPPINESS</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Suffering</t>
+          <t>SUFFERING</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>행복과 고통은 반비례</t>
+        <v>-0.5</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>HAPPINESS 상승 시 SUFFERING 하락</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Suffering</t>
+          <t>SUFFERING</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Happiness</t>
+          <t>HAPPINESS</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>고통과 행복은 반비례</t>
+        <v>-0.5</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>SUFFERING 상승 시 HAPPINESS 하락</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Inventory</t>
+          <t>INVENTORY</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Money</t>
+          <t>MONEY</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>재고가 많으면 돈 감소</t>
+        <v>-0.5</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>INVENTORY 상승 시 MONEY 하락</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Staff_Fatigue</t>
+          <t>STAFF_FATIGUE</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>REPUTATION</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.25</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>피로도가 높으면 평판 감소</t>
+        <v>-0.5</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>STAFF_FATIGUE 상승 시 REPUTATION 하락</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Facility</t>
+          <t>STAFF_FATIGUE</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Money</t>
+          <t>FACILITY</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.15</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>시설이 좋으면 돈 감소</t>
+        <v>-0.5</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>STAFF_FATIGUE 상승 시 FACILITY 하락</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Demand</t>
+          <t>FACILITY</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Inventory</t>
+          <t>MONEY</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.2</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>수요가 높으면 재고 감소</t>
+        <v>-0.5</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>FACILITY 상승 시 MONEY 하락</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Money</t>
+          <t>DEMAND</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Facility</t>
+          <t>INVENTORY</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.4</v>
+        <v>-0.5</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>-{PROBABILITY_LOW_THRESHOLD} - 0.1</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>돈이 많을수록 시설 투자 (동적 계산)</t>
+          <t>DEMAND 상승 시 INVENTORY 하락</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>DEMAND</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Demand</t>
+          <t>STAFF_FATIGUE</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.35</v>
+        <v>-0.5</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>{PROBABILITY_LOW_THRESHOLD} + 0.05</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>평판이 높을수록 수요 증가 (동적 계산)</t>
+          <t>DEMAND 상승 시 STAFF_FATIGUE 하락</t>
         </is>
       </c>
     </row>
@@ -1683,7 +2799,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1704,11 +2820,6 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Formula</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
           <t>Description</t>
         </is>
       </c>
@@ -1716,47 +2827,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Money</t>
+          <t>MONEY</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{PROBABILITY_LOW_THRESHOLD} - 0.1</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>돈이 많을수록 위험 증가 (동적)</t>
+          <t>MONEY의 불확실성 가중치</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>REPUTATION</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{PROBABILITY_LOW_THRESHOLD} * 0.5</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>평판이 높을수록 기대치 상승으로 위험 (동적)</t>
+          <t>REPUTATION의 불확실성 가중치</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Happiness</t>
+          <t>HAPPINESS</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1764,19 +2865,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>-{PROBABILITY_LOW_THRESHOLD} / 3</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>행복이 높을수록 위험 감소 (동적)</t>
+          <t>HAPPINESS의 불확실성 가중치</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Suffering</t>
+          <t>SUFFERING</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1784,72 +2880,67 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{PROBABILITY_LOW_THRESHOLD} - 0.1</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>고통이 높을수록 위험 증가 (동적)</t>
+          <t>SUFFERING의 불확실성 가중치</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Inventory</t>
+          <t>INVENTORY</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>0.05</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>재고가 많을수록 약간 위험</t>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>INVENTORY의 불확실성 가중치</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Staff_Fatigue</t>
+          <t>STAFF_FATIGUE</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>0.15</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>직원 피로도가 높을수록 위험</t>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>STAFF_FATIGUE의 불확실성 가중치</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Facility</t>
+          <t>FACILITY</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>-0.2</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>시설 상태가 좋을수록 위험 감소</t>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>FACILITY의 불확실성 가중치</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Demand</t>
+          <t>DEMAND</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>0.1</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>수요가 높을수록 약간 위험</t>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>DEMAND의 불확실성 가중치</t>
         </is>
       </c>
     </row>
@@ -3567,245 +4658,113 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="29" customWidth="1" min="1" max="1"/>
-    <col width="9" customWidth="1" min="2" max="2"/>
-    <col width="7" customWidth="1" min="3" max="3"/>
-    <col width="16" customWidth="1" min="4" max="4"/>
-    <col width="17" customWidth="1" min="5" max="5"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Key</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Category</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>TEST_MONEY</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="n">
-        <v>20000</v>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>float</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>테스트용 자금</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>test_data</t>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TEST_MIN_CASCADE_EVENTS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>testing</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>최소 연쇄 효과 메시지 수</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TEST_REPUTATION</t>
+          <t>TEST_EXPECTED_EVENTS</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>테스트용 평판</t>
+          <t>testing</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>test_data</t>
+          <t>예상 이벤트 수</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>TEST_HAPPINESS</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>float</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>테스트용 행복도</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>test_data</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>TEST_MIN_CASCADE_EVENTS</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>TEST_METRICS_HISTORY_LENGTH</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>int</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>최소 연쇄 효과 메시지 수</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>test_validation</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>TEST_EXPECTED_EVENTS</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>예상 이벤트 수</t>
-        </is>
-      </c>
-      <c r="E6" s="3" t="inlineStr">
-        <is>
-          <t>test_validation</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>TEST_METRICS_HISTORY_LENGTH</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>testing</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>메트릭 히스토리 길이</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>test_validation</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="inlineStr">
-        <is>
-          <t>MAX_RETRY_ATTEMPTS</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>최대 재시도 횟수</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="inlineStr">
-        <is>
-          <t>test_config</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>TIMEOUT_SECONDS</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>float</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>재시도 간 대기 시간(초)</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>test_config</t>
         </is>
       </c>
     </row>

</xml_diff>